<commit_message>
[LaraParser] Adds parser for StringLiteral
</commit_message>
<xml_diff>
--- a/LaraParser/EsprimaNodes.xlsx
+++ b/LaraParser/EsprimaNodes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>Node</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>StringLiteral</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -613,17 +616,17 @@
   <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +640,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -647,385 +650,391 @@
       </c>
       <c r="E2" s="3">
         <f>(COUNTA(B:B)-1)/$D$2</f>
-        <v>1.2987012987012988E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.896103896103896E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>74</v>
       </c>

</xml_diff>